<commit_message>
Lab 02 - part 2
</commit_message>
<xml_diff>
--- a/Laboratorio 2/Risultati.xlsx
+++ b/Laboratorio 2/Risultati.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s326834_studenti_polito_it/Documents/Corsi attuali/Image Processing and Computer vision/laboratori/Laboratorio 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5453F98D-11FB-46AC-8043-054105FA9FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{5453F98D-11FB-46AC-8043-054105FA9FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F079987F-3F72-4A36-9A64-35CF88F42FCF}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{1E9CE8D4-49AF-4B1B-BD4A-13DCAD5A8B28}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Altezza px</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Telefono_zoom</t>
+  </si>
+  <si>
+    <t>MTF oggettivo</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2EA46C-2AAA-45EF-94E7-2F61DAA2A509}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:M25"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -553,7 +556,7 @@
         <v>4.7748691099476437</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:L5" si="0">C3/C4</f>
+        <f t="shared" ref="C5:E5" si="0">C3/C4</f>
         <v>4.7665505226480835</v>
       </c>
       <c r="D5" s="3">
@@ -591,7 +594,7 @@
         <v>350</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:L7" si="1">100*C6</f>
+        <f t="shared" ref="C7:E7" si="1">100*C6</f>
         <v>350</v>
       </c>
       <c r="D7" s="1">
@@ -612,7 +615,7 @@
         <v>1671.2041884816754</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:L8" si="2">C7*C5</f>
+        <f t="shared" ref="C8:E8" si="2">C7*C5</f>
         <v>1668.2926829268292</v>
       </c>
       <c r="D8" s="4">
@@ -633,7 +636,7 @@
         <v>2736</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ref="C9:L9" si="3">C3</f>
+        <f t="shared" ref="C9:E9" si="3">C3</f>
         <v>2736</v>
       </c>
       <c r="D9" s="1">
@@ -654,7 +657,7 @@
         <v>0.61082024432809767</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" ref="C10:L10" si="4">C8/C9</f>
+        <f t="shared" ref="C10:E10" si="4">C8/C9</f>
         <v>0.6097560975609756</v>
       </c>
       <c r="D10" s="3">
@@ -750,6 +753,10 @@
       <c r="E17" s="1">
         <v>3.25</v>
       </c>
+      <c r="G17" s="1">
+        <f>G18/100</f>
+        <v>2.4384000000000001</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
@@ -771,6 +778,10 @@
         <f t="shared" ref="E18" si="10">100*E17</f>
         <v>325</v>
       </c>
+      <c r="G18" s="1">
+        <f>G19/B16</f>
+        <v>243.84</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
@@ -793,7 +804,10 @@
         <v>1203.2025620496397</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4">
+        <f>B23*B20</f>
+        <v>1167.3600000000001</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -809,7 +823,7 @@
         <v>3648</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ref="C20:L20" si="14">C14</f>
+        <f t="shared" ref="C20:E20" si="14">C14</f>
         <v>3648</v>
       </c>
       <c r="D20" s="1">
@@ -849,6 +863,14 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>